<commit_message>
Update the expected outcome column to reflected the latest review labels from geneticists that were used during validation.
</commit_message>
<xml_diff>
--- a/configs/files/publication_params_validation.xlsx
+++ b/configs/files/publication_params_validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyeonshin/Documents/AI-Projects/ai-genetics-functional-paper/configs/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F174E67-79DE-5344-9B6B-CCD5E4FF63A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065759B0-CABB-E641-9ED6-6ED9E23C230B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38040" yWindow="-620" windowWidth="39540" windowHeight="24240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_parameters" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="362">
   <si>
     <t>id</t>
   </si>
@@ -222,9 +222,6 @@
     <t>CFTR</t>
   </si>
   <si>
-    <t>pub-18</t>
-  </si>
-  <si>
     <t>Analysis of Trafficking, Stability and Function of Human Connexin 26 Gap Junction Channels with Deafness-Causing Mutations in the Fourth Transmembrane Helix.pdf</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
   </si>
   <si>
     <t>pub-20</t>
-  </si>
-  <si>
-    <t>c.212G&gt;A (p.G71E)</t>
   </si>
   <si>
     <t>pub-21</t>
@@ -645,21 +639,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>A&gt;G,GLA c.376A&gt;G (p.Ser126Gly),NM_000169.3:c.376A&gt;G,NC_000023.11:g.101401803T&gt;C,Ser126Gly,LRG_672p1:p.(S126G),NP_000160.1:p.(Ser126Gly),S126G,p.Ser126Gly,NP_000160.1:p.(S126G),p.S126G,(Ser126Gly),NC_000023.10:g.100656791T&gt;C,376A/G,(S126G),GLA c.376A&gt;G,c.376A&gt;G,p.(Ser126Gly),LRG_672p1:p.(Ser126Gly),p.(S126G),c.376A/G</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NC_000023.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10:g.38226678G&gt;A,OTC c.212G&gt;A,212G&gt;A,NP_000522.3:p.(G71E),p.(G71E),212G/A,c.212G&gt;A,(G71E),(Gly71Glu),p.G71E,LRG_846p1:p.(Gly71Glu),G71E,NM_000531.6:c.212G&gt;A,p.Gly71Glu,p.(Gly71Glu),LRG_846p1:p.(G71E),OTC c.212G&gt;A (p.Gly71Glu),Gly71Glu,c.212G/A,NP_000522.3:p.(Gly71Glu),NC_000023.11:g.38367425G&gt;A</t>
     </r>
   </si>
   <si>
@@ -2355,16 +2334,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="110.1640625" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
@@ -2387,10 +2366,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2398,10 +2377,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -2410,10 +2389,10 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2421,7 +2400,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -2433,10 +2412,10 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2444,7 +2423,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -2456,10 +2435,10 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2467,7 +2446,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -2479,10 +2458,10 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2490,7 +2469,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -2502,10 +2481,10 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2513,7 +2492,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -2525,10 +2504,10 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2536,7 +2515,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -2548,10 +2527,10 @@
         <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2559,7 +2538,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -2571,10 +2550,10 @@
         <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2582,10 +2561,10 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>39</v>
@@ -2594,10 +2573,10 @@
         <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2605,10 +2584,10 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
@@ -2617,10 +2596,10 @@
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2628,7 +2607,7 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
@@ -2640,10 +2619,10 @@
         <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2651,10 +2630,10 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>46</v>
@@ -2663,10 +2642,10 @@
         <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2674,7 +2653,7 @@
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>50</v>
@@ -2686,10 +2665,10 @@
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2697,7 +2676,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
@@ -2709,10 +2688,10 @@
         <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2720,10 +2699,10 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>58</v>
@@ -2732,10 +2711,10 @@
         <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2743,22 +2722,22 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" t="s">
         <v>62</v>
       </c>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2766,68 +2745,68 @@
         <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" t="s">
         <v>66</v>
       </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2835,283 +2814,283 @@
         <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" t="s">
-        <v>90</v>
-      </c>
       <c r="F24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" t="s">
-        <v>105</v>
-      </c>
       <c r="F28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E31" t="s">
-        <v>116</v>
-      </c>
-      <c r="F31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>154</v>
       </c>
+      <c r="E31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="G31" s="6" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>159</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>160</v>
@@ -3120,44 +3099,44 @@
         <v>161</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>165</v>
+        <v>59</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>166</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>280</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>167</v>
@@ -3166,44 +3145,44 @@
         <v>168</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>172</v>
+        <v>36</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>173</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>174</v>
@@ -3212,67 +3191,67 @@
         <v>175</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>36</v>
+        <v>176</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E39" s="2" t="s">
         <v>183</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>184</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>185</v>
@@ -3281,21 +3260,21 @@
         <v>186</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>187</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>188</v>
@@ -3304,44 +3283,44 @@
         <v>189</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>193</v>
+        <v>70</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>194</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>195</v>
@@ -3350,21 +3329,21 @@
         <v>196</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>197</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>198</v>
@@ -3373,458 +3352,458 @@
         <v>199</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>72</v>
+        <v>200</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E48" s="3" t="s">
         <v>215</v>
       </c>
+      <c r="E48" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="F48" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E50" s="4" t="s">
         <v>223</v>
       </c>
+      <c r="E50" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="F50" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E52" s="5" t="s">
         <v>231</v>
       </c>
+      <c r="E52" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="F52" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E53" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="E53" s="5" t="s">
+        <v>236</v>
+      </c>
       <c r="F53" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>239</v>
+        <v>32</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>240</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>32</v>
+      <c r="E55" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B56" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>275</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>276</v>
@@ -3833,243 +3812,220 @@
         <v>277</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B66" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B71" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B72" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B73" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>357</v>
-      </c>
-      <c r="B74" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -4091,10 +4047,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4102,7 +4058,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4110,15 +4066,15 @@
         <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4126,7 +4082,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4134,7 +4090,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -4142,7 +4098,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4150,23 +4106,23 @@
         <v>34</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4174,15 +4130,15 @@
         <v>45</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4190,7 +4146,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -4198,479 +4154,479 @@
         <v>54</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update publication id column to use the latest.
</commit_message>
<xml_diff>
--- a/configs/files/publication_params_validation.xlsx
+++ b/configs/files/publication_params_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyeonshin/Documents/AI-Projects/ai-genetics-functional-paper/configs/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065759B0-CABB-E641-9ED6-6ED9E23C230B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631941D0-8AE5-6247-BA9D-7A9828EE93DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38040" yWindow="-620" windowWidth="39540" windowHeight="24240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38620" yWindow="300" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_parameters" sheetId="1" r:id="rId1"/>
@@ -1428,9 +1428,6 @@
     <t>pub-72</t>
   </si>
   <si>
-    <t>pub-73</t>
-  </si>
-  <si>
     <t>Pathogenic</t>
   </si>
   <si>
@@ -1450,6 +1447,9 @@
   </si>
   <si>
     <t>Distinct effects of single amino-acid changes to tuberin on the function of the tuberin‚Äìhamartin complex.pdf</t>
+  </si>
+  <si>
+    <t>pub-18</t>
   </si>
 </sst>
 </file>
@@ -2336,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:XFD62"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2392,7 +2392,7 @@
         <v>152</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2415,7 +2415,7 @@
         <v>125</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2438,7 +2438,7 @@
         <v>126</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2461,7 +2461,7 @@
         <v>127</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2484,7 +2484,7 @@
         <v>128</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2507,7 +2507,7 @@
         <v>129</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2530,7 +2530,7 @@
         <v>130</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2553,7 +2553,7 @@
         <v>131</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2576,7 +2576,7 @@
         <v>132</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2599,7 +2599,7 @@
         <v>133</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2622,7 +2622,7 @@
         <v>134</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2645,7 +2645,7 @@
         <v>134</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2668,7 +2668,7 @@
         <v>135</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2691,7 +2691,7 @@
         <v>136</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2714,7 +2714,7 @@
         <v>137</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2737,7 +2737,7 @@
         <v>138</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2760,12 +2760,12 @@
         <v>139</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>361</v>
       </c>
       <c r="B19" t="s">
         <v>124</v>
@@ -2783,12 +2783,12 @@
         <v>140</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
         <v>124</v>
@@ -2806,12 +2806,12 @@
         <v>141</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>124</v>
@@ -2829,12 +2829,12 @@
         <v>142</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>124</v>
@@ -2852,12 +2852,12 @@
         <v>143</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>124</v>
@@ -2875,12 +2875,12 @@
         <v>144</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
         <v>124</v>
@@ -2898,12 +2898,12 @@
         <v>145</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
         <v>124</v>
@@ -2921,12 +2921,12 @@
         <v>146</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
         <v>124</v>
@@ -2944,12 +2944,12 @@
         <v>147</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
         <v>124</v>
@@ -2967,12 +2967,12 @@
         <v>148</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
         <v>124</v>
@@ -2990,12 +2990,12 @@
         <v>149</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
         <v>124</v>
@@ -3013,12 +3013,12 @@
         <v>150</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
         <v>124</v>
@@ -3036,12 +3036,12 @@
         <v>151</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
         <v>124</v>
@@ -3059,12 +3059,12 @@
         <v>156</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
         <v>124</v>
@@ -3082,12 +3082,12 @@
         <v>159</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
@@ -3105,12 +3105,12 @@
         <v>163</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
         <v>124</v>
@@ -3128,12 +3128,12 @@
         <v>166</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>280</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
         <v>124</v>
@@ -3151,12 +3151,12 @@
         <v>170</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B36" t="s">
         <v>124</v>
@@ -3174,12 +3174,12 @@
         <v>173</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B37" t="s">
         <v>124</v>
@@ -3197,12 +3197,12 @@
         <v>177</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B38" t="s">
         <v>124</v>
@@ -3220,12 +3220,12 @@
         <v>181</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B39" t="s">
         <v>124</v>
@@ -3243,12 +3243,12 @@
         <v>184</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B40" t="s">
         <v>124</v>
@@ -3266,12 +3266,12 @@
         <v>187</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B41" t="s">
         <v>124</v>
@@ -3289,12 +3289,12 @@
         <v>191</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B42" t="s">
         <v>124</v>
@@ -3312,12 +3312,12 @@
         <v>194</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B43" t="s">
         <v>124</v>
@@ -3335,12 +3335,12 @@
         <v>197</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B44" t="s">
         <v>124</v>
@@ -3358,12 +3358,12 @@
         <v>201</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B45" t="s">
         <v>124</v>
@@ -3381,12 +3381,12 @@
         <v>205</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B46" t="s">
         <v>124</v>
@@ -3404,12 +3404,12 @@
         <v>209</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B47" t="s">
         <v>124</v>
@@ -3427,12 +3427,12 @@
         <v>213</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B48" t="s">
         <v>124</v>
@@ -3450,12 +3450,12 @@
         <v>217</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B49" t="s">
         <v>124</v>
@@ -3473,12 +3473,12 @@
         <v>221</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B50" t="s">
         <v>124</v>
@@ -3496,12 +3496,12 @@
         <v>225</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B51" t="s">
         <v>124</v>
@@ -3519,12 +3519,12 @@
         <v>229</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B52" t="s">
         <v>124</v>
@@ -3542,12 +3542,12 @@
         <v>233</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B53" t="s">
         <v>124</v>
@@ -3565,12 +3565,12 @@
         <v>237</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B54" t="s">
         <v>124</v>
@@ -3588,12 +3588,12 @@
         <v>240</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B55" t="s">
         <v>124</v>
@@ -3611,12 +3611,12 @@
         <v>244</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B56" t="s">
         <v>124</v>
@@ -3634,12 +3634,12 @@
         <v>248</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B57" t="s">
         <v>124</v>
@@ -3657,12 +3657,12 @@
         <v>252</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B58" t="s">
         <v>124</v>
@@ -3680,12 +3680,12 @@
         <v>256</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B59" t="s">
         <v>124</v>
@@ -3703,12 +3703,12 @@
         <v>260</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B60" t="s">
         <v>124</v>
@@ -3726,12 +3726,12 @@
         <v>264</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B61" t="s">
         <v>124</v>
@@ -3749,12 +3749,12 @@
         <v>268</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B62" t="s">
         <v>124</v>
@@ -3772,12 +3772,12 @@
         <v>272</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B63" t="s">
         <v>124</v>
@@ -3795,12 +3795,12 @@
         <v>275</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B64" t="s">
         <v>124</v>
@@ -3818,12 +3818,12 @@
         <v>279</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B65" t="s">
         <v>124</v>
@@ -3841,12 +3841,12 @@
         <v>284</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B66" t="s">
         <v>124</v>
@@ -3864,12 +3864,12 @@
         <v>289</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B67" t="s">
         <v>124</v>
@@ -3887,12 +3887,12 @@
         <v>294</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B68" t="s">
         <v>124</v>
@@ -3910,12 +3910,12 @@
         <v>299</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B69" t="s">
         <v>124</v>
@@ -3933,12 +3933,12 @@
         <v>304</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B70" t="s">
         <v>124</v>
@@ -3956,12 +3956,12 @@
         <v>309</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B71" t="s">
         <v>124</v>
@@ -3979,12 +3979,12 @@
         <v>314</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B72" t="s">
         <v>124</v>
@@ -4002,12 +4002,12 @@
         <v>319</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B73" t="s">
         <v>124</v>
@@ -4025,7 +4025,7 @@
         <v>325</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -4050,7 +4050,7 @@
         <v>121</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4058,7 +4058,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4066,15 +4066,15 @@
         <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4082,7 +4082,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4090,7 +4090,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -4098,7 +4098,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4106,7 +4106,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4114,7 +4114,7 @@
         <v>123</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4122,7 +4122,7 @@
         <v>119</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4130,7 +4130,7 @@
         <v>45</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4138,7 +4138,7 @@
         <v>120</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4146,7 +4146,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -4154,7 +4154,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -4162,7 +4162,7 @@
         <v>118</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -4170,7 +4170,7 @@
         <v>60</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -4178,7 +4178,7 @@
         <v>64</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4186,7 +4186,7 @@
         <v>122</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -4194,7 +4194,7 @@
         <v>117</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -4202,7 +4202,7 @@
         <v>73</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -4210,7 +4210,7 @@
         <v>78</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -4218,7 +4218,7 @@
         <v>82</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -4226,15 +4226,15 @@
         <v>86</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -4242,7 +4242,7 @@
         <v>93</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -4250,7 +4250,7 @@
         <v>97</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -4258,7 +4258,7 @@
         <v>101</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -4266,7 +4266,7 @@
         <v>105</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -4274,7 +4274,7 @@
         <v>108</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -4282,7 +4282,7 @@
         <v>112</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -4290,7 +4290,7 @@
         <v>153</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -4298,7 +4298,7 @@
         <v>157</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -4306,7 +4306,7 @@
         <v>160</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -4314,7 +4314,7 @@
         <v>164</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -4322,7 +4322,7 @@
         <v>167</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -4330,7 +4330,7 @@
         <v>171</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -4338,7 +4338,7 @@
         <v>174</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -4346,7 +4346,7 @@
         <v>178</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -4354,7 +4354,7 @@
         <v>182</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -4362,7 +4362,7 @@
         <v>185</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -4370,7 +4370,7 @@
         <v>188</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -4378,7 +4378,7 @@
         <v>192</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -4386,7 +4386,7 @@
         <v>195</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -4394,7 +4394,7 @@
         <v>198</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -4402,7 +4402,7 @@
         <v>202</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -4410,7 +4410,7 @@
         <v>206</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -4418,7 +4418,7 @@
         <v>210</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -4426,7 +4426,7 @@
         <v>214</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -4434,7 +4434,7 @@
         <v>218</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -4442,7 +4442,7 @@
         <v>222</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -4450,7 +4450,7 @@
         <v>226</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -4458,7 +4458,7 @@
         <v>230</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -4466,7 +4466,7 @@
         <v>234</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -4474,7 +4474,7 @@
         <v>238</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -4482,7 +4482,7 @@
         <v>241</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -4490,7 +4490,7 @@
         <v>245</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -4498,7 +4498,7 @@
         <v>249</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -4506,7 +4506,7 @@
         <v>253</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -4514,7 +4514,7 @@
         <v>257</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -4522,7 +4522,7 @@
         <v>261</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -4530,7 +4530,7 @@
         <v>265</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -4538,7 +4538,7 @@
         <v>269</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -4546,7 +4546,7 @@
         <v>273</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -4554,7 +4554,7 @@
         <v>276</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -4562,7 +4562,7 @@
         <v>281</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -4570,7 +4570,7 @@
         <v>286</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -4578,7 +4578,7 @@
         <v>291</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -4586,7 +4586,7 @@
         <v>296</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -4594,7 +4594,7 @@
         <v>301</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -4602,7 +4602,7 @@
         <v>306</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -4610,7 +4610,7 @@
         <v>311</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -4618,7 +4618,7 @@
         <v>316</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -4626,7 +4626,7 @@
         <v>322</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>